<commit_message>
March 8, 2021,Payment sheet update
</commit_message>
<xml_diff>
--- a/Payment sheet.xlsx
+++ b/Payment sheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="66">
   <si>
     <t>Invoice Overdue</t>
   </si>
@@ -205,6 +205,18 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>Advanced</t>
+  </si>
+  <si>
+    <t>The Nainital Bank Ltd.</t>
+  </si>
+  <si>
+    <t>Axis Bank Ltd.</t>
   </si>
 </sst>
 </file>
@@ -263,7 +275,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -300,8 +312,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -361,20 +379,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -384,24 +393,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -425,16 +416,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -448,23 +433,43 @@
     <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill patternType="gray125">
@@ -774,11 +779,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:S59"/>
+  <dimension ref="A2:X73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
+      <pane ySplit="5" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -799,33 +804,34 @@
     <col min="16" max="16" width="15.42578125" customWidth="1"/>
     <col min="17" max="17" width="14.28515625" customWidth="1"/>
     <col min="19" max="19" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:19" ht="27" customHeight="1">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:24" ht="27" customHeight="1">
+      <c r="A2" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="9"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="39"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="12"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="42"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:19">
-      <c r="A3" s="37"/>
+    <row r="3" spans="1:24">
+      <c r="A3" s="29"/>
       <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
@@ -844,10 +850,16 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
-      <c r="S3" s="2"/>
-    </row>
-    <row r="4" spans="1:19">
-      <c r="A4" s="38"/>
+      <c r="S3" s="31"/>
+      <c r="W3" t="s">
+        <v>20</v>
+      </c>
+      <c r="X3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
+      <c r="A4" s="30"/>
       <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
@@ -866,8 +878,15 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
-    </row>
-    <row r="5" spans="1:19" ht="45" customHeight="1">
+      <c r="S4" s="31"/>
+      <c r="W4" t="s">
+        <v>62</v>
+      </c>
+      <c r="X4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="45" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
@@ -919,142 +938,153 @@
       <c r="Q5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="S5" s="29"/>
-    </row>
-    <row r="6" spans="1:19">
-      <c r="A6" s="33" t="s">
+      <c r="S5" s="32"/>
+      <c r="W5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
+      <c r="A6" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="35">
+      <c r="C6" s="27">
         <v>44026</v>
       </c>
-      <c r="D6" s="34">
+      <c r="D6" s="26">
         <v>3843</v>
       </c>
-      <c r="E6" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="34">
+      <c r="E6" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="26">
         <v>659703</v>
       </c>
-      <c r="G6" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="H6" s="35">
+      <c r="G6" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="H6" s="27">
         <v>44068</v>
       </c>
-      <c r="I6" s="35"/>
-      <c r="J6" s="34">
+      <c r="I6" s="27"/>
+      <c r="J6" s="26">
         <v>5227</v>
       </c>
-      <c r="K6" s="35">
+      <c r="K6" s="27">
         <v>44068</v>
       </c>
-      <c r="L6" s="34"/>
-      <c r="M6" s="34"/>
-      <c r="N6" s="34"/>
-      <c r="O6" s="34"/>
-      <c r="P6" s="34"/>
-      <c r="Q6" s="34" t="str">
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
+      <c r="Q6" s="26" t="str">
         <f>IF(L6=0,"NO","YES")</f>
         <v>NO</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
-      <c r="A7" s="33" t="s">
+    <row r="7" spans="1:24">
+      <c r="A7" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="35">
+      <c r="C7" s="27">
         <v>44037</v>
       </c>
-      <c r="D7" s="34">
+      <c r="D7" s="26">
         <v>1652</v>
       </c>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="34"/>
-      <c r="K7" s="34"/>
-      <c r="L7" s="34"/>
-      <c r="M7" s="34"/>
-      <c r="N7" s="34"/>
-      <c r="O7" s="34"/>
-      <c r="P7" s="34"/>
-      <c r="Q7" s="34"/>
-    </row>
-    <row r="8" spans="1:19">
-      <c r="A8" s="33" t="s">
+      <c r="E7" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="26"/>
+      <c r="O7" s="26"/>
+      <c r="P7" s="26"/>
+      <c r="Q7" s="26"/>
+    </row>
+    <row r="8" spans="1:24">
+      <c r="A8" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="35">
+      <c r="C8" s="27">
         <v>44037</v>
       </c>
-      <c r="D8" s="34">
+      <c r="D8" s="26">
         <v>1357</v>
       </c>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="34"/>
-      <c r="K8" s="34"/>
-      <c r="L8" s="34"/>
-      <c r="M8" s="34"/>
-      <c r="N8" s="34"/>
-      <c r="O8" s="34"/>
-      <c r="P8" s="34"/>
-      <c r="Q8" s="34"/>
-    </row>
-    <row r="9" spans="1:19">
-      <c r="A9" s="33" t="s">
+      <c r="E8" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="26"/>
+      <c r="O8" s="26"/>
+      <c r="P8" s="26"/>
+      <c r="Q8" s="26"/>
+    </row>
+    <row r="9" spans="1:24">
+      <c r="A9" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="35">
+      <c r="C9" s="27">
         <v>44040</v>
       </c>
-      <c r="D9" s="34">
+      <c r="D9" s="26">
         <v>1841</v>
       </c>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="34"/>
-      <c r="L9" s="34"/>
-      <c r="M9" s="34"/>
-      <c r="N9" s="34"/>
-      <c r="O9" s="34"/>
-      <c r="P9" s="34"/>
-      <c r="Q9" s="34"/>
-    </row>
-    <row r="10" spans="1:19">
-      <c r="A10" s="16"/>
+      <c r="E9" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="26"/>
+      <c r="N9" s="26"/>
+      <c r="O9" s="26"/>
+      <c r="P9" s="26"/>
+      <c r="Q9" s="26"/>
+    </row>
+    <row r="10" spans="1:24">
+      <c r="A10" s="10"/>
       <c r="B10" s="2"/>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="21" t="s">
         <v>61</v>
       </c>
       <c r="D10" s="2">
         <f>SUM(D6:D9)</f>
         <v>8693</v>
       </c>
-      <c r="E10" s="2"/>
+      <c r="E10" s="26" t="s">
+        <v>20</v>
+      </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -1068,20 +1098,22 @@
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
     </row>
-    <row r="11" spans="1:19">
-      <c r="A11" s="17" t="s">
+    <row r="11" spans="1:24">
+      <c r="A11" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C11" s="6">
         <v>44026</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="7">
         <v>104548</v>
       </c>
-      <c r="E11" s="2"/>
+      <c r="E11" s="26" t="s">
+        <v>20</v>
+      </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -1095,11 +1127,11 @@
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
     </row>
-    <row r="12" spans="1:19">
-      <c r="A12" s="17" t="s">
+    <row r="12" spans="1:24">
+      <c r="A12" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C12" s="6">
@@ -1108,7 +1140,9 @@
       <c r="D12" s="2">
         <v>87792</v>
       </c>
-      <c r="E12" s="2"/>
+      <c r="E12" s="26" t="s">
+        <v>20</v>
+      </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -1122,11 +1156,11 @@
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
     </row>
-    <row r="13" spans="1:19">
-      <c r="A13" s="17" t="s">
+    <row r="13" spans="1:24">
+      <c r="A13" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="6">
@@ -1135,7 +1169,9 @@
       <c r="D13" s="2">
         <v>396952</v>
       </c>
-      <c r="E13" s="2"/>
+      <c r="E13" s="26" t="s">
+        <v>20</v>
+      </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -1149,11 +1185,11 @@
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
     </row>
-    <row r="14" spans="1:19">
-      <c r="A14" s="17" t="s">
+    <row r="14" spans="1:24">
+      <c r="A14" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C14" s="6">
@@ -1162,7 +1198,9 @@
       <c r="D14" s="2">
         <v>98176</v>
       </c>
-      <c r="E14" s="2"/>
+      <c r="E14" s="26" t="s">
+        <v>20</v>
+      </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -1176,11 +1214,11 @@
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
     </row>
-    <row r="15" spans="1:19">
-      <c r="A15" s="17" t="s">
+    <row r="15" spans="1:24">
+      <c r="A15" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C15" s="6">
@@ -1189,7 +1227,9 @@
       <c r="D15" s="2">
         <v>118236</v>
       </c>
-      <c r="E15" s="2"/>
+      <c r="E15" s="26" t="s">
+        <v>20</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -1203,11 +1243,11 @@
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
     </row>
-    <row r="16" spans="1:19">
-      <c r="A16" s="17" t="s">
+    <row r="16" spans="1:24">
+      <c r="A16" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C16" s="6">
@@ -1216,7 +1256,9 @@
       <c r="D16" s="2">
         <v>220660</v>
       </c>
-      <c r="E16" s="2"/>
+      <c r="E16" s="26" t="s">
+        <v>20</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -1231,10 +1273,10 @@
       <c r="Q16" s="2"/>
     </row>
     <row r="17" spans="1:17">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C17" s="6">
@@ -1243,7 +1285,9 @@
       <c r="D17" s="2">
         <v>221745.6</v>
       </c>
-      <c r="E17" s="2"/>
+      <c r="E17" s="26" t="s">
+        <v>20</v>
+      </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -1258,10 +1302,10 @@
       <c r="Q17" s="2"/>
     </row>
     <row r="18" spans="1:17">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C18" s="6">
@@ -1270,7 +1314,9 @@
       <c r="D18" s="2">
         <v>677556</v>
       </c>
-      <c r="E18" s="2"/>
+      <c r="E18" s="26" t="s">
+        <v>20</v>
+      </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -1285,10 +1331,10 @@
       <c r="Q18" s="2"/>
     </row>
     <row r="19" spans="1:17">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C19" s="6">
@@ -1297,7 +1343,9 @@
       <c r="D19" s="2">
         <v>168504</v>
       </c>
-      <c r="E19" s="2"/>
+      <c r="E19" s="26" t="s">
+        <v>20</v>
+      </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -1312,7 +1360,7 @@
       <c r="Q19" s="2"/>
     </row>
     <row r="20" spans="1:17">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="10" t="s">
         <v>37</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -1324,7 +1372,9 @@
       <c r="D20" s="2">
         <v>5313.54</v>
       </c>
-      <c r="E20" s="2"/>
+      <c r="E20" s="26" t="s">
+        <v>20</v>
+      </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
@@ -1339,7 +1389,7 @@
       <c r="Q20" s="2"/>
     </row>
     <row r="21" spans="1:17">
-      <c r="A21" s="16">
+      <c r="A21" s="10">
         <v>200</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -1351,7 +1401,9 @@
       <c r="D21" s="2">
         <v>1045.48</v>
       </c>
-      <c r="E21" s="2"/>
+      <c r="E21" s="26" t="s">
+        <v>20</v>
+      </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -1366,10 +1418,10 @@
       <c r="Q21" s="2"/>
     </row>
     <row r="22" spans="1:17">
-      <c r="A22" s="16">
+      <c r="A22" s="10">
         <v>176</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="9" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="6">
@@ -1378,7 +1430,9 @@
       <c r="D22" s="2">
         <v>5428</v>
       </c>
-      <c r="E22" s="2"/>
+      <c r="E22" s="26" t="s">
+        <v>20</v>
+      </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -1393,10 +1447,10 @@
       <c r="Q22" s="2"/>
     </row>
     <row r="23" spans="1:17">
-      <c r="A23" s="16">
+      <c r="A23" s="10">
         <v>56</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="9" t="s">
         <v>40</v>
       </c>
       <c r="C23" s="6">
@@ -1405,7 +1459,9 @@
       <c r="D23" s="2">
         <v>85862.7</v>
       </c>
-      <c r="E23" s="2"/>
+      <c r="E23" s="26" t="s">
+        <v>20</v>
+      </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
@@ -1420,205 +1476,219 @@
       <c r="Q23" s="2"/>
     </row>
     <row r="24" spans="1:17">
-      <c r="A24" s="30" t="s">
+      <c r="A24" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="32">
+      <c r="C24" s="24">
         <v>44050</v>
       </c>
-      <c r="D24" s="31">
+      <c r="D24" s="23">
         <v>1239</v>
       </c>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="31"/>
-      <c r="J24" s="31"/>
-      <c r="K24" s="31"/>
-      <c r="L24" s="31"/>
-      <c r="M24" s="31"/>
-      <c r="N24" s="31"/>
-      <c r="O24" s="31"/>
-      <c r="P24" s="31"/>
-      <c r="Q24" s="31"/>
+      <c r="E24" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="23"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="23"/>
+      <c r="O24" s="23"/>
+      <c r="P24" s="23"/>
+      <c r="Q24" s="23"/>
     </row>
     <row r="25" spans="1:17">
-      <c r="A25" s="30" t="s">
+      <c r="A25" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="31" t="s">
+      <c r="B25" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="32">
+      <c r="C25" s="24">
         <v>44051</v>
       </c>
-      <c r="D25" s="31">
+      <c r="D25" s="23">
         <v>1652</v>
       </c>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="31"/>
-      <c r="I25" s="31"/>
-      <c r="J25" s="31"/>
-      <c r="K25" s="31"/>
-      <c r="L25" s="31"/>
-      <c r="M25" s="31"/>
-      <c r="N25" s="31"/>
-      <c r="O25" s="31"/>
-      <c r="P25" s="31"/>
-      <c r="Q25" s="31"/>
+      <c r="E25" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="23"/>
+      <c r="L25" s="23"/>
+      <c r="M25" s="23"/>
+      <c r="N25" s="23"/>
+      <c r="O25" s="23"/>
+      <c r="P25" s="23"/>
+      <c r="Q25" s="23"/>
     </row>
     <row r="26" spans="1:17">
-      <c r="A26" s="30" t="s">
+      <c r="A26" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="31" t="s">
+      <c r="B26" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="32">
+      <c r="C26" s="24">
         <v>44053</v>
       </c>
-      <c r="D26" s="31">
+      <c r="D26" s="23">
         <v>1126</v>
       </c>
-      <c r="E26" s="31"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="31"/>
-      <c r="I26" s="31"/>
-      <c r="J26" s="31"/>
-      <c r="K26" s="31"/>
-      <c r="L26" s="31"/>
-      <c r="M26" s="31"/>
-      <c r="N26" s="31"/>
-      <c r="O26" s="31"/>
-      <c r="P26" s="31"/>
-      <c r="Q26" s="31"/>
+      <c r="E26" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="23"/>
+      <c r="K26" s="23"/>
+      <c r="L26" s="23"/>
+      <c r="M26" s="23"/>
+      <c r="N26" s="23"/>
+      <c r="O26" s="23"/>
+      <c r="P26" s="23"/>
+      <c r="Q26" s="23"/>
     </row>
     <row r="27" spans="1:17">
-      <c r="A27" s="30" t="s">
+      <c r="A27" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="31" t="s">
+      <c r="B27" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="36">
+      <c r="C27" s="28">
         <v>44055</v>
       </c>
-      <c r="D27" s="31">
+      <c r="D27" s="23">
         <v>5227</v>
       </c>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
-      <c r="K27" s="31"/>
-      <c r="L27" s="31"/>
-      <c r="M27" s="31"/>
-      <c r="N27" s="31"/>
-      <c r="O27" s="31"/>
-      <c r="P27" s="31"/>
-      <c r="Q27" s="31"/>
+      <c r="E27" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="23"/>
+      <c r="K27" s="23"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="23"/>
+      <c r="N27" s="23"/>
+      <c r="O27" s="23"/>
+      <c r="P27" s="23"/>
+      <c r="Q27" s="23"/>
     </row>
     <row r="28" spans="1:17">
-      <c r="A28" s="30" t="s">
+      <c r="A28" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="31" t="s">
+      <c r="B28" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="36">
+      <c r="C28" s="28">
         <v>44060</v>
       </c>
-      <c r="D28" s="31">
+      <c r="D28" s="23">
         <v>1221.3</v>
       </c>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="31"/>
-      <c r="J28" s="31"/>
-      <c r="K28" s="31"/>
-      <c r="L28" s="31"/>
-      <c r="M28" s="31"/>
-      <c r="N28" s="31"/>
-      <c r="O28" s="31"/>
-      <c r="P28" s="31"/>
-      <c r="Q28" s="31"/>
+      <c r="E28" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="23"/>
+      <c r="L28" s="23"/>
+      <c r="M28" s="23"/>
+      <c r="N28" s="23"/>
+      <c r="O28" s="23"/>
+      <c r="P28" s="23"/>
+      <c r="Q28" s="23"/>
     </row>
     <row r="29" spans="1:17">
-      <c r="A29" s="30" t="s">
+      <c r="A29" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="B29" s="31" t="s">
+      <c r="B29" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="C29" s="32">
+      <c r="C29" s="24">
         <v>44068</v>
       </c>
-      <c r="D29" s="31">
+      <c r="D29" s="23">
         <v>2195</v>
       </c>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="31"/>
-      <c r="J29" s="31"/>
-      <c r="K29" s="31"/>
-      <c r="L29" s="31"/>
-      <c r="M29" s="31"/>
-      <c r="N29" s="31"/>
-      <c r="O29" s="31"/>
-      <c r="P29" s="31"/>
-      <c r="Q29" s="31"/>
+      <c r="E29" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23"/>
+      <c r="K29" s="23"/>
+      <c r="L29" s="23"/>
+      <c r="M29" s="23"/>
+      <c r="N29" s="23"/>
+      <c r="O29" s="23"/>
+      <c r="P29" s="23"/>
+      <c r="Q29" s="23"/>
     </row>
     <row r="30" spans="1:17">
-      <c r="A30" s="30" t="s">
+      <c r="A30" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="B30" s="31" t="s">
+      <c r="B30" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="C30" s="36">
+      <c r="C30" s="28">
         <v>44074</v>
       </c>
-      <c r="D30" s="31">
+      <c r="D30" s="23">
         <v>5720.64</v>
       </c>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
-      <c r="K30" s="31"/>
-      <c r="L30" s="31"/>
-      <c r="M30" s="31"/>
-      <c r="N30" s="31"/>
-      <c r="O30" s="31"/>
-      <c r="P30" s="31"/>
-      <c r="Q30" s="31"/>
+      <c r="E30" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="23"/>
+      <c r="K30" s="23"/>
+      <c r="L30" s="23"/>
+      <c r="M30" s="23"/>
+      <c r="N30" s="23"/>
+      <c r="O30" s="23"/>
+      <c r="P30" s="23"/>
+      <c r="Q30" s="23"/>
     </row>
     <row r="31" spans="1:17">
-      <c r="A31" s="25"/>
+      <c r="A31" s="19"/>
       <c r="B31" s="2"/>
-      <c r="C31" s="19" t="s">
+      <c r="C31" s="13" t="s">
         <v>61</v>
       </c>
       <c r="D31" s="2">
         <f>SUM(D24:D30)</f>
         <v>18380.939999999999</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="E31" s="26" t="s">
         <v>20</v>
       </c>
       <c r="F31" s="2">
@@ -1647,7 +1717,7 @@
       </c>
     </row>
     <row r="32" spans="1:17">
-      <c r="A32" s="16"/>
+      <c r="A32" s="10"/>
       <c r="B32" s="2" t="s">
         <v>49</v>
       </c>
@@ -1657,7 +1727,9 @@
       <c r="D32" s="2">
         <v>210000</v>
       </c>
-      <c r="E32" s="2"/>
+      <c r="E32" s="26" t="s">
+        <v>20</v>
+      </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
@@ -1672,19 +1744,21 @@
       <c r="Q32" s="2"/>
     </row>
     <row r="33" spans="1:17">
-      <c r="A33" s="24" t="s">
+      <c r="A33" s="18" t="s">
         <v>51</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="19">
+      <c r="C33" s="13">
         <v>44055</v>
       </c>
       <c r="D33" s="2">
         <v>163312</v>
       </c>
-      <c r="E33" s="2"/>
+      <c r="E33" s="26" t="s">
+        <v>20</v>
+      </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
@@ -1699,19 +1773,21 @@
       <c r="Q33" s="2"/>
     </row>
     <row r="34" spans="1:17">
-      <c r="A34" s="27" t="s">
+      <c r="A34" s="20" t="s">
         <v>52</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C34" s="19">
+      <c r="C34" s="13">
         <v>44059</v>
       </c>
       <c r="D34" s="2">
         <v>302552</v>
       </c>
-      <c r="E34" s="2"/>
+      <c r="E34" s="26" t="s">
+        <v>20</v>
+      </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
@@ -1726,19 +1802,21 @@
       <c r="Q34" s="2"/>
     </row>
     <row r="35" spans="1:17">
-      <c r="A35" s="27" t="s">
+      <c r="A35" s="20" t="s">
         <v>50</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C35" s="19">
+      <c r="C35" s="13">
         <v>44069</v>
       </c>
       <c r="D35" s="2">
         <v>134992</v>
       </c>
-      <c r="E35" s="2"/>
+      <c r="E35" s="26" t="s">
+        <v>20</v>
+      </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
@@ -1753,19 +1831,21 @@
       <c r="Q35" s="2"/>
     </row>
     <row r="36" spans="1:17">
-      <c r="A36" s="25">
+      <c r="A36" s="19">
         <v>1367</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="19">
+      <c r="C36" s="13">
         <v>44069</v>
       </c>
-      <c r="D36" s="22">
+      <c r="D36" s="16">
         <v>2400</v>
       </c>
-      <c r="E36" s="2"/>
+      <c r="E36" s="26" t="s">
+        <v>20</v>
+      </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
@@ -1780,61 +1860,65 @@
       <c r="Q36" s="2"/>
     </row>
     <row r="37" spans="1:17">
-      <c r="A37" s="25">
+      <c r="A37" s="33">
         <v>225</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C37" s="19">
+      <c r="C37" s="13">
         <v>44064</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D37" s="2">
         <v>1888</v>
       </c>
-      <c r="E37" s="2"/>
-      <c r="F37" s="3"/>
+      <c r="E37" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F37" s="2"/>
       <c r="G37" s="2"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
-      <c r="M37" s="3"/>
-      <c r="N37" s="3"/>
-      <c r="O37" s="3"/>
-      <c r="P37" s="3"/>
-      <c r="Q37" s="3"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2"/>
     </row>
     <row r="38" spans="1:17">
-      <c r="A38" s="26">
+      <c r="A38" s="34">
         <v>282</v>
       </c>
-      <c r="B38" s="15" t="s">
+      <c r="B38" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C38" s="23">
+      <c r="C38" s="17">
         <v>282</v>
       </c>
       <c r="D38" s="2">
         <v>1880.92</v>
       </c>
-      <c r="E38" s="2"/>
+      <c r="E38" s="26" t="s">
+        <v>20</v>
+      </c>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="3"/>
-      <c r="L38" s="3"/>
-      <c r="M38" s="3"/>
-      <c r="N38" s="3"/>
-      <c r="O38" s="3"/>
-      <c r="P38" s="3"/>
-      <c r="Q38" s="3"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="2"/>
     </row>
     <row r="39" spans="1:17">
-      <c r="A39" s="16" t="s">
+      <c r="A39" s="35" t="s">
         <v>57</v>
       </c>
       <c r="B39" s="2" t="s">
@@ -1846,415 +1930,675 @@
       <c r="D39" s="2">
         <v>29500</v>
       </c>
-      <c r="E39" s="2"/>
-      <c r="F39" s="22"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
-      <c r="K39" s="3"/>
-      <c r="L39" s="3"/>
-      <c r="M39" s="3"/>
-      <c r="N39" s="3"/>
-      <c r="O39" s="3"/>
-      <c r="P39" s="3"/>
-      <c r="Q39" s="3"/>
+      <c r="E39" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F39" s="16"/>
+      <c r="G39" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2"/>
     </row>
     <row r="40" spans="1:17">
-      <c r="A40" s="25">
+      <c r="A40" s="33">
         <v>240</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C40" s="19">
+      <c r="C40" s="13">
         <v>44074</v>
       </c>
       <c r="D40" s="2">
         <v>15930</v>
       </c>
-      <c r="E40" s="2"/>
-      <c r="F40" s="22"/>
+      <c r="E40" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F40" s="16"/>
       <c r="G40" s="2"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
-      <c r="K40" s="3"/>
-      <c r="L40" s="3"/>
-      <c r="M40" s="3"/>
-      <c r="N40" s="3"/>
-      <c r="O40" s="3"/>
-      <c r="P40" s="3"/>
-      <c r="Q40" s="3"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+      <c r="P40" s="2"/>
+      <c r="Q40" s="2"/>
     </row>
     <row r="41" spans="1:17">
-      <c r="A41" s="25">
+      <c r="A41" s="33">
         <v>5</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C41" s="19">
+      <c r="C41" s="13">
         <v>44059</v>
       </c>
       <c r="D41" s="2">
         <v>48300</v>
       </c>
-      <c r="E41" s="2"/>
+      <c r="E41" s="26" t="s">
+        <v>20</v>
+      </c>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
-      <c r="K41" s="3"/>
-      <c r="L41" s="3"/>
-      <c r="M41" s="3"/>
-      <c r="N41" s="3"/>
-      <c r="O41" s="3"/>
-      <c r="P41" s="3"/>
-      <c r="Q41" s="3"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="2"/>
+      <c r="P41" s="2"/>
+      <c r="Q41" s="2"/>
     </row>
     <row r="42" spans="1:17">
-      <c r="A42" s="16"/>
-      <c r="B42" s="20"/>
+      <c r="A42" s="35"/>
+      <c r="B42" s="14"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
-      <c r="K42" s="3"/>
-      <c r="L42" s="3"/>
-      <c r="M42" s="3"/>
-      <c r="N42" s="3"/>
-      <c r="O42" s="3"/>
-      <c r="P42" s="3"/>
-      <c r="Q42" s="3"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+      <c r="O42" s="2"/>
+      <c r="P42" s="2"/>
+      <c r="Q42" s="2"/>
     </row>
     <row r="43" spans="1:17">
-      <c r="A43" s="18"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
+      <c r="A43" s="12"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
       <c r="G43" s="2"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3"/>
-      <c r="K43" s="3"/>
-      <c r="L43" s="3"/>
-      <c r="M43" s="3"/>
-      <c r="N43" s="3"/>
-      <c r="O43" s="3"/>
-      <c r="P43" s="3"/>
-      <c r="Q43" s="3"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+      <c r="P43" s="2"/>
+      <c r="Q43" s="2"/>
     </row>
     <row r="44" spans="1:17">
-      <c r="A44" s="16"/>
-      <c r="B44" s="19"/>
-      <c r="C44" s="21"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="15"/>
       <c r="D44" s="2"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="22"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="16"/>
       <c r="G44" s="2"/>
-      <c r="H44" s="3"/>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
-      <c r="K44" s="3"/>
-      <c r="L44" s="3"/>
-      <c r="M44" s="3"/>
-      <c r="N44" s="3"/>
-      <c r="O44" s="3"/>
-      <c r="P44" s="3"/>
-      <c r="Q44" s="3"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2"/>
+      <c r="P44" s="2"/>
+      <c r="Q44" s="2"/>
     </row>
     <row r="45" spans="1:17">
-      <c r="A45" s="16"/>
+      <c r="A45" s="35"/>
       <c r="B45" s="6"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
-      <c r="I45" s="3"/>
-      <c r="J45" s="3"/>
-      <c r="K45" s="3"/>
-      <c r="L45" s="3"/>
-      <c r="M45" s="3"/>
-      <c r="N45" s="3"/>
-      <c r="O45" s="3"/>
-      <c r="P45" s="3"/>
-      <c r="Q45" s="3"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+      <c r="O45" s="2"/>
+      <c r="P45" s="2"/>
+      <c r="Q45" s="2"/>
     </row>
     <row r="46" spans="1:17">
-      <c r="A46" s="16"/>
-      <c r="B46" s="19"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
-      <c r="I46" s="3"/>
-      <c r="J46" s="3"/>
-      <c r="K46" s="3"/>
-      <c r="L46" s="3"/>
-      <c r="M46" s="3"/>
-      <c r="N46" s="3"/>
-      <c r="O46" s="3"/>
-      <c r="P46" s="3"/>
-      <c r="Q46" s="3"/>
+      <c r="A46" s="35"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+      <c r="O46" s="2"/>
+      <c r="P46" s="2"/>
+      <c r="Q46" s="2"/>
     </row>
     <row r="47" spans="1:17">
-      <c r="A47" s="16"/>
-      <c r="B47" s="19"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="3"/>
-      <c r="I47" s="3"/>
-      <c r="J47" s="3"/>
-      <c r="K47" s="3"/>
-      <c r="L47" s="3"/>
-      <c r="M47" s="3"/>
-      <c r="N47" s="3"/>
-      <c r="O47" s="3"/>
-      <c r="P47" s="3"/>
-      <c r="Q47" s="3"/>
+      <c r="A47" s="35"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+      <c r="O47" s="2"/>
+      <c r="P47" s="2"/>
+      <c r="Q47" s="2"/>
     </row>
     <row r="48" spans="1:17">
-      <c r="A48" s="16"/>
-      <c r="B48" s="19"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
-      <c r="I48" s="3"/>
-      <c r="J48" s="3"/>
-      <c r="K48" s="3"/>
-      <c r="L48" s="3"/>
-      <c r="M48" s="3"/>
-      <c r="N48" s="3"/>
-      <c r="O48" s="3"/>
-      <c r="P48" s="3"/>
-      <c r="Q48" s="3"/>
+      <c r="A48" s="35"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
+      <c r="O48" s="2"/>
+      <c r="P48" s="2"/>
+      <c r="Q48" s="2"/>
     </row>
     <row r="49" spans="1:17">
-      <c r="A49" s="16"/>
-      <c r="B49" s="19"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-      <c r="I49" s="3"/>
-      <c r="J49" s="3"/>
-      <c r="K49" s="3"/>
-      <c r="L49" s="3"/>
-      <c r="M49" s="3"/>
-      <c r="N49" s="3"/>
-      <c r="O49" s="3"/>
-      <c r="P49" s="3"/>
-      <c r="Q49" s="3"/>
+      <c r="A49" s="35"/>
+      <c r="B49" s="13"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+      <c r="N49" s="2"/>
+      <c r="O49" s="2"/>
+      <c r="P49" s="2"/>
+      <c r="Q49" s="2"/>
     </row>
     <row r="50" spans="1:17">
-      <c r="A50" s="16"/>
-      <c r="B50" s="19"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
-      <c r="I50" s="3"/>
-      <c r="J50" s="3"/>
-      <c r="K50" s="3"/>
-      <c r="L50" s="3"/>
-      <c r="M50" s="3"/>
-      <c r="N50" s="3"/>
-      <c r="O50" s="3"/>
-      <c r="P50" s="3"/>
-      <c r="Q50" s="3"/>
+      <c r="A50" s="35"/>
+      <c r="B50" s="13"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
+      <c r="O50" s="2"/>
+      <c r="P50" s="2"/>
+      <c r="Q50" s="2"/>
     </row>
     <row r="51" spans="1:17">
-      <c r="A51" s="18"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
-      <c r="K51" s="3"/>
-      <c r="L51" s="3"/>
-      <c r="M51" s="3"/>
-      <c r="N51" s="3"/>
-      <c r="O51" s="3"/>
-      <c r="P51" s="3"/>
-      <c r="Q51" s="3"/>
+      <c r="A51" s="12"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+      <c r="L51" s="2"/>
+      <c r="M51" s="2"/>
+      <c r="N51" s="2"/>
+      <c r="O51" s="2"/>
+      <c r="P51" s="2"/>
+      <c r="Q51" s="2"/>
     </row>
     <row r="52" spans="1:17">
-      <c r="A52" s="18"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
-      <c r="H52" s="3"/>
-      <c r="I52" s="3"/>
-      <c r="J52" s="3"/>
-      <c r="K52" s="3"/>
-      <c r="L52" s="3"/>
-      <c r="M52" s="3"/>
-      <c r="N52" s="3"/>
-      <c r="O52" s="3"/>
-      <c r="P52" s="3"/>
-      <c r="Q52" s="3"/>
+      <c r="A52" s="12"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
+      <c r="L52" s="2"/>
+      <c r="M52" s="2"/>
+      <c r="N52" s="2"/>
+      <c r="O52" s="2"/>
+      <c r="P52" s="2"/>
+      <c r="Q52" s="2"/>
     </row>
     <row r="53" spans="1:17">
-      <c r="A53" s="18"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
-      <c r="H53" s="3"/>
-      <c r="I53" s="3"/>
-      <c r="J53" s="3"/>
-      <c r="K53" s="3"/>
-      <c r="L53" s="3"/>
-      <c r="M53" s="3"/>
-      <c r="N53" s="3"/>
-      <c r="O53" s="3"/>
-      <c r="P53" s="3"/>
-      <c r="Q53" s="3"/>
+      <c r="A53" s="12"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2"/>
+      <c r="L53" s="2"/>
+      <c r="M53" s="2"/>
+      <c r="N53" s="2"/>
+      <c r="O53" s="2"/>
+      <c r="P53" s="2"/>
+      <c r="Q53" s="2"/>
     </row>
     <row r="54" spans="1:17">
-      <c r="A54" s="18"/>
-      <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
-      <c r="H54" s="3"/>
-      <c r="I54" s="3"/>
-      <c r="J54" s="3"/>
-      <c r="K54" s="3"/>
-      <c r="L54" s="3"/>
-      <c r="M54" s="3"/>
-      <c r="N54" s="3"/>
-      <c r="O54" s="3"/>
-      <c r="P54" s="3"/>
-      <c r="Q54" s="3"/>
+      <c r="A54" s="12"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
+      <c r="K54" s="2"/>
+      <c r="L54" s="2"/>
+      <c r="M54" s="2"/>
+      <c r="N54" s="2"/>
+      <c r="O54" s="2"/>
+      <c r="P54" s="2"/>
+      <c r="Q54" s="2"/>
     </row>
     <row r="55" spans="1:17">
-      <c r="A55" s="18"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3"/>
-      <c r="H55" s="3"/>
-      <c r="I55" s="3"/>
-      <c r="J55" s="3"/>
-      <c r="K55" s="3"/>
-      <c r="L55" s="3"/>
-      <c r="M55" s="3"/>
-      <c r="N55" s="3"/>
-      <c r="O55" s="3"/>
-      <c r="P55" s="3"/>
-      <c r="Q55" s="3"/>
+      <c r="A55" s="12"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+      <c r="K55" s="2"/>
+      <c r="L55" s="2"/>
+      <c r="M55" s="2"/>
+      <c r="N55" s="2"/>
+      <c r="O55" s="2"/>
+      <c r="P55" s="2"/>
+      <c r="Q55" s="2"/>
     </row>
     <row r="56" spans="1:17">
-      <c r="A56" s="18"/>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
-      <c r="G56" s="3"/>
-      <c r="H56" s="3"/>
-      <c r="I56" s="3"/>
-      <c r="J56" s="3"/>
-      <c r="K56" s="3"/>
-      <c r="L56" s="3"/>
-      <c r="M56" s="3"/>
-      <c r="N56" s="3"/>
-      <c r="O56" s="3"/>
-      <c r="P56" s="3"/>
-      <c r="Q56" s="3"/>
+      <c r="A56" s="12"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+      <c r="K56" s="2"/>
+      <c r="L56" s="2"/>
+      <c r="M56" s="2"/>
+      <c r="N56" s="2"/>
+      <c r="O56" s="2"/>
+      <c r="P56" s="2"/>
+      <c r="Q56" s="2"/>
     </row>
     <row r="57" spans="1:17">
-      <c r="A57" s="18"/>
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3"/>
-      <c r="H57" s="3"/>
-      <c r="I57" s="3"/>
-      <c r="J57" s="3"/>
-      <c r="K57" s="3"/>
-      <c r="L57" s="3"/>
-      <c r="M57" s="3"/>
-      <c r="N57" s="3"/>
-      <c r="O57" s="3"/>
-      <c r="P57" s="3"/>
-      <c r="Q57" s="3"/>
+      <c r="A57" s="12"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
+      <c r="K57" s="2"/>
+      <c r="L57" s="2"/>
+      <c r="M57" s="2"/>
+      <c r="N57" s="2"/>
+      <c r="O57" s="2"/>
+      <c r="P57" s="2"/>
+      <c r="Q57" s="2"/>
     </row>
     <row r="58" spans="1:17">
-      <c r="A58" s="18"/>
-      <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="3"/>
-      <c r="F58" s="3"/>
-      <c r="G58" s="3"/>
-      <c r="H58" s="3"/>
-      <c r="I58" s="3"/>
-      <c r="J58" s="3"/>
-      <c r="K58" s="3"/>
-      <c r="L58" s="3"/>
-      <c r="M58" s="3"/>
-      <c r="N58" s="3"/>
-      <c r="O58" s="3"/>
-      <c r="P58" s="3"/>
-      <c r="Q58" s="3"/>
+      <c r="A58" s="12"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+      <c r="J58" s="2"/>
+      <c r="K58" s="2"/>
+      <c r="L58" s="2"/>
+      <c r="M58" s="2"/>
+      <c r="N58" s="2"/>
+      <c r="O58" s="2"/>
+      <c r="P58" s="2"/>
+      <c r="Q58" s="2"/>
     </row>
     <row r="59" spans="1:17">
       <c r="A59" s="3"/>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="3"/>
-      <c r="F59" s="3"/>
-      <c r="G59" s="3"/>
-      <c r="H59" s="3"/>
-      <c r="I59" s="3"/>
-      <c r="J59" s="3"/>
-      <c r="K59" s="3"/>
-      <c r="L59" s="3"/>
-      <c r="M59" s="3"/>
-      <c r="N59" s="3"/>
-      <c r="O59" s="3"/>
-      <c r="P59" s="3"/>
-      <c r="Q59" s="3"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2"/>
+      <c r="K59" s="2"/>
+      <c r="L59" s="2"/>
+      <c r="M59" s="2"/>
+      <c r="N59" s="2"/>
+      <c r="O59" s="2"/>
+      <c r="P59" s="2"/>
+      <c r="Q59" s="2"/>
+    </row>
+    <row r="60" spans="1:17">
+      <c r="B60" s="36"/>
+      <c r="C60" s="36"/>
+      <c r="D60" s="36"/>
+      <c r="E60" s="36"/>
+      <c r="F60" s="36"/>
+      <c r="G60" s="36"/>
+      <c r="H60" s="36"/>
+      <c r="I60" s="36"/>
+      <c r="J60" s="36"/>
+      <c r="K60" s="36"/>
+      <c r="L60" s="36"/>
+      <c r="M60" s="36"/>
+      <c r="N60" s="36"/>
+      <c r="O60" s="36"/>
+      <c r="P60" s="36"/>
+      <c r="Q60" s="36"/>
+    </row>
+    <row r="61" spans="1:17">
+      <c r="B61" s="36"/>
+      <c r="C61" s="36"/>
+      <c r="D61" s="36"/>
+      <c r="E61" s="36"/>
+      <c r="F61" s="36"/>
+      <c r="G61" s="36"/>
+      <c r="H61" s="36"/>
+      <c r="I61" s="36"/>
+      <c r="J61" s="36"/>
+      <c r="K61" s="36"/>
+      <c r="L61" s="36"/>
+      <c r="M61" s="36"/>
+      <c r="N61" s="36"/>
+      <c r="O61" s="36"/>
+      <c r="P61" s="36"/>
+      <c r="Q61" s="36"/>
+    </row>
+    <row r="62" spans="1:17">
+      <c r="B62" s="36"/>
+      <c r="C62" s="36"/>
+      <c r="D62" s="36"/>
+      <c r="E62" s="36"/>
+      <c r="F62" s="36"/>
+      <c r="G62" s="36"/>
+      <c r="H62" s="36"/>
+      <c r="I62" s="36"/>
+      <c r="J62" s="36"/>
+      <c r="K62" s="36"/>
+      <c r="L62" s="36"/>
+      <c r="M62" s="36"/>
+      <c r="N62" s="36"/>
+      <c r="O62" s="36"/>
+      <c r="P62" s="36"/>
+      <c r="Q62" s="36"/>
+    </row>
+    <row r="63" spans="1:17">
+      <c r="B63" s="36"/>
+      <c r="C63" s="36"/>
+      <c r="D63" s="36"/>
+      <c r="E63" s="36"/>
+      <c r="F63" s="36"/>
+      <c r="G63" s="36"/>
+      <c r="H63" s="36"/>
+      <c r="I63" s="36"/>
+      <c r="J63" s="36"/>
+      <c r="K63" s="36"/>
+      <c r="L63" s="36"/>
+      <c r="M63" s="36"/>
+      <c r="N63" s="36"/>
+      <c r="O63" s="36"/>
+      <c r="P63" s="36"/>
+      <c r="Q63" s="36"/>
+    </row>
+    <row r="64" spans="1:17">
+      <c r="B64" s="36"/>
+      <c r="C64" s="36"/>
+      <c r="D64" s="36"/>
+      <c r="E64" s="36"/>
+      <c r="F64" s="36"/>
+      <c r="G64" s="36"/>
+      <c r="H64" s="36"/>
+      <c r="I64" s="36"/>
+      <c r="J64" s="36"/>
+      <c r="K64" s="36"/>
+      <c r="L64" s="36"/>
+      <c r="M64" s="36"/>
+      <c r="N64" s="36"/>
+      <c r="O64" s="36"/>
+      <c r="P64" s="36"/>
+      <c r="Q64" s="36"/>
+    </row>
+    <row r="65" spans="2:17">
+      <c r="B65" s="36"/>
+      <c r="C65" s="36"/>
+      <c r="D65" s="36"/>
+      <c r="E65" s="36"/>
+      <c r="F65" s="36"/>
+      <c r="G65" s="36"/>
+      <c r="H65" s="36"/>
+      <c r="I65" s="36"/>
+      <c r="J65" s="36"/>
+      <c r="K65" s="36"/>
+      <c r="L65" s="36"/>
+      <c r="M65" s="36"/>
+      <c r="N65" s="36"/>
+      <c r="O65" s="36"/>
+      <c r="P65" s="36"/>
+      <c r="Q65" s="36"/>
+    </row>
+    <row r="66" spans="2:17">
+      <c r="B66" s="36"/>
+      <c r="C66" s="36"/>
+      <c r="D66" s="36"/>
+      <c r="E66" s="36"/>
+      <c r="F66" s="36"/>
+      <c r="G66" s="36"/>
+      <c r="H66" s="36"/>
+      <c r="I66" s="36"/>
+      <c r="J66" s="36"/>
+      <c r="K66" s="36"/>
+      <c r="L66" s="36"/>
+      <c r="M66" s="36"/>
+      <c r="N66" s="36"/>
+      <c r="O66" s="36"/>
+      <c r="P66" s="36"/>
+      <c r="Q66" s="36"/>
+    </row>
+    <row r="67" spans="2:17">
+      <c r="B67" s="36"/>
+      <c r="C67" s="36"/>
+      <c r="D67" s="36"/>
+      <c r="E67" s="36"/>
+      <c r="F67" s="36"/>
+      <c r="G67" s="36"/>
+      <c r="H67" s="36"/>
+      <c r="I67" s="36"/>
+      <c r="J67" s="36"/>
+      <c r="K67" s="36"/>
+      <c r="L67" s="36"/>
+      <c r="M67" s="36"/>
+      <c r="N67" s="36"/>
+      <c r="O67" s="36"/>
+      <c r="P67" s="36"/>
+      <c r="Q67" s="36"/>
+    </row>
+    <row r="68" spans="2:17">
+      <c r="B68" s="36"/>
+      <c r="C68" s="36"/>
+      <c r="D68" s="36"/>
+      <c r="E68" s="36"/>
+      <c r="F68" s="36"/>
+      <c r="G68" s="36"/>
+      <c r="H68" s="36"/>
+      <c r="I68" s="36"/>
+      <c r="J68" s="36"/>
+      <c r="K68" s="36"/>
+      <c r="L68" s="36"/>
+      <c r="M68" s="36"/>
+      <c r="N68" s="36"/>
+      <c r="O68" s="36"/>
+      <c r="P68" s="36"/>
+      <c r="Q68" s="36"/>
+    </row>
+    <row r="69" spans="2:17">
+      <c r="B69" s="36"/>
+      <c r="C69" s="36"/>
+      <c r="D69" s="36"/>
+      <c r="E69" s="36"/>
+      <c r="F69" s="36"/>
+      <c r="G69" s="36"/>
+      <c r="H69" s="36"/>
+      <c r="I69" s="36"/>
+      <c r="J69" s="36"/>
+      <c r="K69" s="36"/>
+      <c r="L69" s="36"/>
+      <c r="M69" s="36"/>
+      <c r="N69" s="36"/>
+      <c r="O69" s="36"/>
+      <c r="P69" s="36"/>
+      <c r="Q69" s="36"/>
+    </row>
+    <row r="70" spans="2:17">
+      <c r="B70" s="36"/>
+      <c r="C70" s="36"/>
+      <c r="D70" s="36"/>
+      <c r="E70" s="36"/>
+      <c r="F70" s="36"/>
+      <c r="G70" s="36"/>
+      <c r="H70" s="36"/>
+      <c r="I70" s="36"/>
+      <c r="J70" s="36"/>
+      <c r="K70" s="36"/>
+      <c r="L70" s="36"/>
+      <c r="M70" s="36"/>
+      <c r="N70" s="36"/>
+      <c r="O70" s="36"/>
+      <c r="P70" s="36"/>
+      <c r="Q70" s="36"/>
+    </row>
+    <row r="71" spans="2:17">
+      <c r="B71" s="36"/>
+      <c r="C71" s="36"/>
+      <c r="D71" s="36"/>
+      <c r="E71" s="36"/>
+      <c r="F71" s="36"/>
+      <c r="G71" s="36"/>
+      <c r="H71" s="36"/>
+      <c r="I71" s="36"/>
+      <c r="J71" s="36"/>
+      <c r="K71" s="36"/>
+      <c r="L71" s="36"/>
+      <c r="M71" s="36"/>
+      <c r="N71" s="36"/>
+      <c r="O71" s="36"/>
+      <c r="P71" s="36"/>
+      <c r="Q71" s="36"/>
+    </row>
+    <row r="72" spans="2:17">
+      <c r="B72" s="36"/>
+      <c r="C72" s="36"/>
+      <c r="D72" s="36"/>
+      <c r="E72" s="36"/>
+      <c r="F72" s="36"/>
+      <c r="G72" s="36"/>
+      <c r="H72" s="36"/>
+      <c r="I72" s="36"/>
+      <c r="J72" s="36"/>
+      <c r="K72" s="36"/>
+      <c r="L72" s="36"/>
+      <c r="M72" s="36"/>
+      <c r="N72" s="36"/>
+      <c r="O72" s="36"/>
+      <c r="P72" s="36"/>
+      <c r="Q72" s="36"/>
+    </row>
+    <row r="73" spans="2:17">
+      <c r="B73" s="36"/>
+      <c r="C73" s="36"/>
+      <c r="D73" s="36"/>
+      <c r="E73" s="36"/>
+      <c r="F73" s="36"/>
+      <c r="G73" s="36"/>
+      <c r="H73" s="36"/>
+      <c r="I73" s="36"/>
+      <c r="J73" s="36"/>
+      <c r="K73" s="36"/>
+      <c r="L73" s="36"/>
+      <c r="M73" s="36"/>
+      <c r="N73" s="36"/>
+      <c r="O73" s="36"/>
+      <c r="P73" s="36"/>
+      <c r="Q73" s="36"/>
     </row>
   </sheetData>
   <autoFilter ref="A5:Q23"/>
@@ -2263,19 +2607,22 @@
     <mergeCell ref="I2:M2"/>
   </mergeCells>
   <conditionalFormatting sqref="Q6">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>IF($L$6=0,"YES","NO")</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>IF($L$6=0,"NO","YES")</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G31 G33:G44">
+      <formula1>$X$3:$X$4</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:E41">
-      <formula1>$S$3:$S$5</formula1>
+      <formula1>$W$3:$W$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G44">
-      <formula1>$S$3:$S$4</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G32">
+      <formula1>$X$3:$X$4</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>